<commit_message>
Atualizao do controle de pneus
</commit_message>
<xml_diff>
--- a/backend/Relatorios/Tabelas/tFABRICANTES.XLSX
+++ b/backend/Relatorios/Tabelas/tFABRICANTES.XLSX
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7c850682481644d/Área de Trabalho/Dados/Manutenção/Dashboard Manutenção/PCM-Hub/backend/Relatorios/Tabelas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_4FE674733814572368F8C35DFC8C3BD8BAB4A661" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C17A66E-1E39-4BF4-8688-F3193E794AE3}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_4FE674733814572368F8C35DFC8C3BD8BAB4A661" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16A48C96-6D7C-4CC8-B8AB-12552251052C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet!$A$1:$B$206</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1598,7 +1601,9 @@
   </sheetPr>
   <dimension ref="A1:B206"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>